<commit_message>
[feature]: hr-manager controller added
</commit_message>
<xml_diff>
--- a/data/generated/employee_leave_applications.xlsx
+++ b/data/generated/employee_leave_applications.xlsx
@@ -1,116 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\JavaScript Projects\leave-management-system\data\generated\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB90B10A-E000-4634-A26C-110EFC8E616F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
-  <si>
-    <t>Leave ID</t>
-  </si>
-  <si>
-    <t>Employee Code</t>
-  </si>
-  <si>
-    <t>Employee Name</t>
-  </si>
-  <si>
-    <t>WhatsApp Number</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Designation</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>Work Location</t>
-  </si>
-  <si>
-    <t>From Date</t>
-  </si>
-  <si>
-    <t>To Date</t>
-  </si>
-  <si>
-    <t>Leave Reason</t>
-  </si>
-  <si>
-    <t>Manager Employee Code</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Submission Date</t>
-  </si>
-  <si>
-    <t>Last Updated</t>
-  </si>
-  <si>
-    <t>LV-1753192917133-EBOH</t>
-  </si>
-  <si>
-    <t>PILLP003</t>
-  </si>
-  <si>
-    <t>Sanjay Dhal</t>
-  </si>
-  <si>
-    <t>dhaljaga192@gmail.com</t>
-  </si>
-  <si>
-    <t>Senior Mechanic</t>
-  </si>
-  <si>
-    <t>Mechanical</t>
-  </si>
-  <si>
-    <t>Raichur</t>
-  </si>
-  <si>
-    <t>02-12-2025</t>
-  </si>
-  <si>
-    <t>07-12-2025</t>
-  </si>
-  <si>
-    <t>For my personal reason</t>
-  </si>
-  <si>
-    <t>PILLP305</t>
-  </si>
-  <si>
-    <t>2025-07-22</t>
-  </si>
-  <si>
-    <t>Manager Approved</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,21 +65,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -479,116 +396,115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="13" max="13" width="20.375" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Leave ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Role</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Employee Code</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Employee Name</v>
+      </c>
+      <c r="E1" t="str">
+        <v>WhatsApp Number</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Designation</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Department</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Work Location</v>
+      </c>
+      <c r="J1" t="str">
+        <v>From Date</v>
+      </c>
+      <c r="K1" t="str">
+        <v>To Date</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Leave Reason</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Manager Employee Code</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Submission Date</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Last Updated</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2">
-        <v>7384731240</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" t="s">
-        <v>26</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v/>
+      </c>
+      <c r="B2" t="str">
+        <v/>
+      </c>
+      <c r="C2" t="str">
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v/>
+      </c>
+      <c r="K2" t="str">
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <v/>
+      </c>
+      <c r="M2" t="str">
+        <v/>
+      </c>
+      <c r="N2" t="str">
+        <v/>
+      </c>
+      <c r="O2" t="str">
+        <v/>
+      </c>
+      <c r="P2" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:O1 A2:L2 N2:O2" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>